<commit_message>
Archon ACI First Release
</commit_message>
<xml_diff>
--- a/archon/locale.xlsx
+++ b/archon/locale.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="60">
   <si>
     <t>ko</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -32,10 +32,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Error</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -44,10 +40,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>success</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Success</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -60,10 +52,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>failed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Failed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -72,39 +60,176 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Request Error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>request error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>요청 오류</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>manager allocation error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Manager Allocation Error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>매니저 할당 오류</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>application error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Application Error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>어플리케이션 오류</t>
+    <t>Create</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>이름</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>암호</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Refresh</t>
+  </si>
+  <si>
+    <t>갱신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>등록</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>상태</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>시스템</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>종류</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>버전</t>
+  </si>
+  <si>
+    <t>Admin ID</t>
+  </si>
+  <si>
+    <t>관리자 ID</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>정보</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>모델</t>
+  </si>
+  <si>
+    <t>MAC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Application</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어플리케이션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manager</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매니저</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요청</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>State</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unknown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알수없음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>운영체제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>End</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종료</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -169,9 +294,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -476,16 +615,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.625" style="1" customWidth="1"/>
-    <col min="2" max="4" width="25.625" customWidth="1"/>
+    <col min="1" max="1" width="25.625" style="3" customWidth="1"/>
+    <col min="2" max="4" width="25.625" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -503,90 +643,407 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D8" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B25" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="C25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
     </row>
   </sheetData>
+  <sortState ref="A2:D29">
+    <sortCondition ref="A2:A29"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>